<commit_message>
[Update] 사망시 dialog 출력
</commit_message>
<xml_diff>
--- a/Assets/Resources/ExcelDB/Dialog.xlsx
+++ b/Assets/Resources/ExcelDB/Dialog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qkrwh\OneDrive\문서\GitHub\IdleSoul\Assets\Resources\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464CA6FA-EBCE-4F3A-A48A-A4953584932A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C6CB81-2A5D-4F35-829D-1CF42973EF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{3E1520F0-0D86-45AB-A9AD-F526B6BD53CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="51">
   <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -207,6 +207,40 @@
   </si>
   <si>
     <t>으아악! 아니야!!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/TalkSprite/Fleur</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플뢰르</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미안.. 갑자기 데자뷰가..</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭐..뭔가? 갑자기…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>겨우 저 정도 적들에게 쓰러지다니..
+내 체면이 말이 아니군…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>본인의 능력치 강화나 스크롤은 제대로 구한건가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우두머리들은 강력하니 그때 만큼은
+직접 몸을 조종하는게 좋을거야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그럼 다시 한 번 가보자고.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -597,7 +631,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1188,7 +1222,7 @@
         <v>3</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" t="s">
         <v>20</v>
@@ -1245,6 +1279,18 @@
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
+        <v>43</v>
+      </c>
+      <c r="J22" t="s">
+        <v>18</v>
+      </c>
       <c r="K22">
         <v>0</v>
       </c>
@@ -1262,11 +1308,23 @@
       <c r="D23">
         <v>1</v>
       </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" t="s">
+        <v>19</v>
+      </c>
       <c r="K23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="33" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1278,6 +1336,18 @@
       </c>
       <c r="D24">
         <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" t="s">
+        <v>18</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1296,11 +1366,23 @@
       <c r="D25">
         <v>1</v>
       </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" t="s">
+        <v>18</v>
+      </c>
       <c r="K25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="33" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1312,6 +1394,18 @@
       </c>
       <c r="D26">
         <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" t="s">
+        <v>18</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1330,6 +1424,18 @@
       <c r="D27">
         <v>1</v>
       </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" t="s">
+        <v>18</v>
+      </c>
       <c r="K27">
         <v>0</v>
       </c>
@@ -1339,10 +1445,10 @@
         <v>24</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1356,10 +1462,10 @@
         <v>25</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1373,10 +1479,10 @@
         <v>26</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D30">
         <v>1</v>

</xml_diff>